<commit_message>
Added new package for TestNG
</commit_message>
<xml_diff>
--- a/target/test-classes/dataDriven/ExcelData.xlsx
+++ b/target/test-classes/dataDriven/ExcelData.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohit_panwar\eclipse-workspace\LearnSelenium\src\test\java\dataDriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{C232DBE1-C477-4DCA-B997-99A52CCD35B9}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89BF17B-4ED7-4EAA-B67B-E3FEFD2B3C15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="RegPage" r:id="rId1" sheetId="1"/>
+    <sheet name="RegPage" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>firstname</t>
   </si>
@@ -88,16 +88,12 @@
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>Status</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -123,7 +119,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -134,11 +130,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="55"/>
       </patternFill>
     </fill>
   </fills>
@@ -152,21 +143,20 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -183,10 +173,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -221,7 +211,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -256,7 +246,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -350,21 +340,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -381,7 +371,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -433,25 +423,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="F1" sqref="F1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -470,9 +460,6 @@
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s" s="3">
-        <v>21</v>
-      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -544,12 +531,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink r:id="rId2" ref="C3" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink r:id="rId3" ref="C4" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink r:id="rId4" ref="C5" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>